<commit_message>
Figure and .xlsx file Updates - includes Proteomics overlaps
1) Updates to reflect changes in presentation/color scheme/ etc. for various figures

2) Proteomics Core Genome analysis similar to Figure 1C (with RNA). No proteins found to change in the same direction amongst the orthologs

3) Added growth analysis - non-essential genes that cause significantly slower growth when deleted from Giaver 2002 were compared to gene age groups
</commit_message>
<xml_diff>
--- a/Figure2/Proteomics_Core_Analysis/yli_proteins_CoreAnalysis.xlsx
+++ b/Figure2/Proteomics_Core_Analysis/yli_proteins_CoreAnalysis.xlsx
@@ -1,28 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doughty/Documents/GitHub/CHASSY_multiOmics_Analysis/Figure2/Proteomics_Core_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5798ED-DA5C-FE4D-9E8B-8CF9CC5534C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2E3693-FF41-3C41-9BFC-A19EF352EF00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35740" yWindow="3520" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35740" yWindow="3520" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yli_Prots_Detected" sheetId="1" r:id="rId1"/>
     <sheet name="yli_SIG_Proteins_HiT_logFC1" sheetId="2" r:id="rId2"/>
     <sheet name="yli_SIG_Proteins_LpH_logFC1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2921" uniqueCount="1728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2966" uniqueCount="1771">
   <si>
     <t>genes</t>
   </si>
@@ -5206,6 +5214,135 @@
   </si>
   <si>
     <t>Total Measured</t>
+  </si>
+  <si>
+    <t>DDR48</t>
+  </si>
+  <si>
+    <t>ACH1</t>
+  </si>
+  <si>
+    <t>DSD1</t>
+  </si>
+  <si>
+    <t>MRPL35</t>
+  </si>
+  <si>
+    <t>GSF2</t>
+  </si>
+  <si>
+    <t>NPL3</t>
+  </si>
+  <si>
+    <t>YML6</t>
+  </si>
+  <si>
+    <t>ARF3</t>
+  </si>
+  <si>
+    <t>YHB1</t>
+  </si>
+  <si>
+    <t>ATH1</t>
+  </si>
+  <si>
+    <t>HSP12</t>
+  </si>
+  <si>
+    <t>AIM2</t>
+  </si>
+  <si>
+    <t>RTC3</t>
+  </si>
+  <si>
+    <t>NIT2</t>
+  </si>
+  <si>
+    <t>MSC1</t>
+  </si>
+  <si>
+    <t>VCX1</t>
+  </si>
+  <si>
+    <t>YDR109C</t>
+  </si>
+  <si>
+    <t>ECM31</t>
+  </si>
+  <si>
+    <t>GPH1</t>
+  </si>
+  <si>
+    <t>INO1</t>
+  </si>
+  <si>
+    <t>ERG6</t>
+  </si>
+  <si>
+    <t>40S ribosomal protein S27</t>
+  </si>
+  <si>
+    <t>PNP1</t>
+  </si>
+  <si>
+    <t>ATG26</t>
+  </si>
+  <si>
+    <t>YME2</t>
+  </si>
+  <si>
+    <t>RSC9</t>
+  </si>
+  <si>
+    <t>CHO2</t>
+  </si>
+  <si>
+    <t>NHP2</t>
+  </si>
+  <si>
+    <t>MRPL4</t>
+  </si>
+  <si>
+    <t>YPR127W</t>
+  </si>
+  <si>
+    <t>YLR173W</t>
+  </si>
+  <si>
+    <t>ECM29</t>
+  </si>
+  <si>
+    <t>PCT1</t>
+  </si>
+  <si>
+    <t>SHB17</t>
+  </si>
+  <si>
+    <t>GLR1</t>
+  </si>
+  <si>
+    <t>ABZ1</t>
+  </si>
+  <si>
+    <t>MCM6</t>
+  </si>
+  <si>
+    <t>VPS33</t>
+  </si>
+  <si>
+    <t>SIL1</t>
+  </si>
+  <si>
+    <t>CDC21</t>
+  </si>
+  <si>
+    <t>IMG1</t>
+  </si>
+  <si>
+    <t>HEM14</t>
+  </si>
+  <si>
+    <t>RTC5</t>
   </si>
 </sst>
 </file>
@@ -6049,8 +6186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1724"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19868,1648 +20005,1795 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="F12:G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C2">
         <v>-2.1918699606255601</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>6.9053476898764496E-23</v>
       </c>
-      <c r="D2" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C3">
+        <v>1.30676346020054</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.24546898873057E-8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C4">
+        <v>1.5051115265892301</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.2330265882767699E-6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1731</v>
+      </c>
+      <c r="C5">
+        <v>-1.63242419882569</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4.6691520286334504E-6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1732</v>
+      </c>
+      <c r="C6">
+        <v>-1.42924470887532</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.7903685394627099E-5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C7">
+        <v>-1.0287284129691301</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2.0425640004120499E-5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C8">
+        <v>-1.4741625757162899</v>
+      </c>
+      <c r="D8">
+        <v>5.6696437914738904E-4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1735</v>
+      </c>
+      <c r="C9">
+        <v>-1.5792760596125499</v>
+      </c>
+      <c r="D9">
+        <v>7.0393864166444205E-4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1726</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1726</v>
+      </c>
+      <c r="H9" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="C10">
         <v>-2.4313283172273898</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D10" s="1">
         <v>2.15856358753696E-19</v>
       </c>
-      <c r="D3" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="E10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G10">
+        <v>1032</v>
+      </c>
+      <c r="H10">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="C11">
         <v>-2.1760118371277399</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D11" s="1">
         <v>2.4529613329764602E-19</v>
       </c>
-      <c r="D4" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="E11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G11">
+        <f>COUNTIF($E:$E,G9)</f>
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <f>COUNTIF($E:$E,H9)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="C12">
         <v>-2.0928554368683399</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D12" s="1">
         <v>1.6710022076633701E-12</v>
       </c>
-      <c r="D5" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>1.40603815746873</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2.0381588694860601E-8</v>
-      </c>
-      <c r="D6" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>1.30676346020054</v>
-      </c>
-      <c r="C7" s="1">
-        <v>4.24546898873057E-8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>-1.5026941975577699</v>
-      </c>
-      <c r="C8" s="1">
-        <v>9.2317367456417298E-7</v>
-      </c>
-      <c r="D8" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>-1.3145255751532601</v>
-      </c>
-      <c r="C9" s="1">
-        <v>9.2317367456417298E-7</v>
-      </c>
-      <c r="D9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1726</v>
-      </c>
-      <c r="G9" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>1.5051115265892301</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1.2330265882767699E-6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1726</v>
-      </c>
-      <c r="F10">
-        <v>1032</v>
-      </c>
-      <c r="G10">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>1.1823854352951699</v>
-      </c>
-      <c r="C11" s="1">
-        <v>4.2109766207079598E-6</v>
-      </c>
-      <c r="D11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F11">
-        <f>COUNTIF($D:$D,F9)</f>
-        <v>8</v>
-      </c>
-      <c r="G11">
-        <f>COUNTIF($D:$D,G9)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>-1.63242419882569</v>
-      </c>
-      <c r="C12" s="1">
-        <v>4.6691520286334504E-6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1726</v>
-      </c>
-      <c r="F12">
-        <f>((F11/F10)*100)</f>
-        <v>0.77519379844961245</v>
+      <c r="E12" t="e">
+        <v>#N/A</v>
       </c>
       <c r="G12">
         <f>((G11/G10)*100)</f>
+        <v>0.77519379844961245</v>
+      </c>
+      <c r="H12">
+        <f>((H11/H10)*100)</f>
         <v>1.4471780028943559</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>-1.42924470887532</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1.7903685394627099E-5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>1.40603815746873</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2.0381588694860601E-8</v>
+      </c>
+      <c r="E13" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>-1.0287284129691301</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2.0425640004120499E-5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>-1.5026941975577699</v>
+      </c>
+      <c r="D14" s="1">
+        <v>9.2317367456417298E-7</v>
+      </c>
+      <c r="E14" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>-1.3145255751532601</v>
+      </c>
+      <c r="D15" s="1">
+        <v>9.2317367456417298E-7</v>
+      </c>
+      <c r="E15" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>1.1823854352951699</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4.2109766207079598E-6</v>
+      </c>
+      <c r="E16" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B15">
+      <c r="C17">
         <v>1.01871734822586</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D17" s="1">
         <v>3.3014419963465201E-5</v>
       </c>
-      <c r="D15" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="E17" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B16">
+      <c r="C18">
         <v>1.1070562647992599</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D18" s="1">
         <v>6.9349053430567699E-5</v>
       </c>
-      <c r="D16" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="E18" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B17">
+      <c r="C19">
         <v>1.092138404318</v>
       </c>
-      <c r="C17">
+      <c r="D19">
         <v>1.5100431105433501E-4</v>
       </c>
-      <c r="D17" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>-1.4741625757162899</v>
-      </c>
-      <c r="C18">
-        <v>5.6696437914738904E-4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>-1.5792760596125499</v>
-      </c>
-      <c r="C19">
-        <v>7.0393864166444205E-4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1726</v>
+      <c r="E19" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E19">
+    <sortCondition ref="E2:E19"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="F12:G12"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2">
-        <v>-3.5045135684935498</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.32233603142404E-55</v>
-      </c>
-      <c r="D2" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1275</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C2">
+        <v>2.1913427817122102</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3.14019041059767E-21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1320</v>
-      </c>
-      <c r="B3">
-        <v>-2.2868103650932898</v>
-      </c>
-      <c r="C3" s="1">
-        <v>8.5489467789449903E-27</v>
-      </c>
-      <c r="D3" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>475</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C3">
+        <v>-2.2556588966035398</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9.0783033635441297E-18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>922</v>
-      </c>
-      <c r="B4">
-        <v>-2.1334658367813901</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3.64159475163907E-23</v>
-      </c>
-      <c r="D4" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>752</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C4">
+        <v>-1.86037036723702</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3.54368218655103E-13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>323</v>
-      </c>
-      <c r="B5">
-        <v>2.3515349720062502</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4.6938835034542499E-23</v>
-      </c>
-      <c r="D5" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>437</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C5">
+        <v>1.4858975462087101</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4.8448382750820595E-13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1275</v>
-      </c>
-      <c r="B6">
-        <v>2.1913427817122102</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3.14019041059767E-21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1061</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C6">
+        <v>-1.7821926576200899</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.9614278014944399E-12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>293</v>
-      </c>
-      <c r="B7">
-        <v>2.0779405387146701</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6.1338979533654301E-21</v>
-      </c>
-      <c r="D7" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C7">
+        <v>-1.3288272014720399</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.62658080002992E-11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>-2.2821387380741198</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3.2624775540480903E-20</v>
-      </c>
-      <c r="D8" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C8">
+        <v>-2.8796573881859402</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7.7775395089806197E-11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B9">
-        <v>-2.8898049751989499</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.35382887594342E-18</v>
-      </c>
-      <c r="D9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1726</v>
-      </c>
-      <c r="G9" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1552</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C9">
+        <v>-2.0438599888878599</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2.4220508604906199E-9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1726</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1726</v>
+      </c>
+      <c r="H9" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>475</v>
-      </c>
-      <c r="B10">
-        <v>-2.2556588966035398</v>
-      </c>
-      <c r="C10" s="1">
-        <v>9.0783033635441297E-18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1726</v>
-      </c>
-      <c r="F10">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C10">
+        <v>-1.99255488807799</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2.59906964508959E-9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1726</v>
+      </c>
+      <c r="G10">
         <v>1032</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>691</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>-1.7747004413554299</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3.0528707945058897E-17</v>
-      </c>
-      <c r="D11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F11">
-        <f>COUNTIF($D:$D,F9)</f>
+        <v>189</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C11">
+        <v>-1.1799194610025201</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5.09438515353527E-8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1726</v>
+      </c>
+      <c r="G11">
+        <f>COUNTIF($E:$E,G9)</f>
         <v>37</v>
       </c>
-      <c r="G11">
-        <f>COUNTIF($D:$D,G9)</f>
+      <c r="H11">
+        <f>COUNTIF($E:$E,H9)</f>
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12">
-        <v>-1.55591553622964</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3.0528707945058897E-17</v>
-      </c>
-      <c r="D12" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F12">
-        <f>((F11/F10)*100)</f>
-        <v>3.5852713178294575</v>
+        <v>224</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C12">
+        <v>1.2461051126032201</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.5011477666384201E-7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1726</v>
       </c>
       <c r="G12">
         <f>((G11/G10)*100)</f>
+        <v>3.5852713178294575</v>
+      </c>
+      <c r="H12">
+        <f>((H11/H10)*100)</f>
         <v>7.9594790159189577</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C13">
+        <v>-1.2234421781558</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3.9373922751673799E-7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C14">
+        <v>1.0679696345156799</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4.0667927823455498E-7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C15">
+        <v>1.0524700752590199</v>
+      </c>
+      <c r="D15" s="1">
+        <v>9.4937485745716404E-7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C16">
+        <v>1.46455562637854</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3.0289792320679399E-6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>271</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1750</v>
+      </c>
+      <c r="C17">
+        <v>1.1959200342032299</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3.55628518913805E-6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C18">
+        <v>-1.0847203408766299</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.7155248462453598E-5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C19">
+        <v>-1.0217631192591801</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2.3916407570055301E-5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1753</v>
+      </c>
+      <c r="C20">
+        <v>2.3235159089566499</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3.04325258625224E-5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C21">
+        <v>1.0204416778493699</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3.3520452137941403E-5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1755</v>
+      </c>
+      <c r="C22">
+        <v>-1.12822436758008</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3.6756536668956703E-5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C23">
+        <v>1.1432972758036</v>
+      </c>
+      <c r="D23" s="1">
+        <v>4.0796203427487102E-5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C24">
+        <v>1.0317782244409299</v>
+      </c>
+      <c r="D24" s="1">
+        <v>7.1645079986050697E-5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C25">
+        <v>-1.3779073656566301</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7.6231238054967797E-5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>847</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C26">
+        <v>-1.1815399713377399</v>
+      </c>
+      <c r="D26" s="1">
+        <v>9.2788717779559198E-5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>968</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C27">
+        <v>1.0039694740943701</v>
+      </c>
+      <c r="D27">
+        <v>1.23455357134426E-4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C28">
+        <v>-1.0422139202433001</v>
+      </c>
+      <c r="D28">
+        <v>1.3178587082486701E-4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C29">
+        <v>-1.0052650095943401</v>
+      </c>
+      <c r="D29">
+        <v>1.6277017857066399E-4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C30">
+        <v>-1.00373648914888</v>
+      </c>
+      <c r="D30">
+        <v>2.8586141165042798E-4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>440</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1763</v>
+      </c>
+      <c r="C31">
+        <v>-1.1173923333012199</v>
+      </c>
+      <c r="D31">
+        <v>2.86633308770816E-4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>439</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1764</v>
+      </c>
+      <c r="C32">
+        <v>-1.47176509312627</v>
+      </c>
+      <c r="D32">
+        <v>6.4021010615734897E-4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1765</v>
+      </c>
+      <c r="C33">
+        <v>-1.04689807204282</v>
+      </c>
+      <c r="D33">
+        <v>7.7577589121875497E-4</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1766</v>
+      </c>
+      <c r="C34">
+        <v>1.06762679466085</v>
+      </c>
+      <c r="D34">
+        <v>8.5783220937633105E-4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C35">
+        <v>-1.3034555548731801</v>
+      </c>
+      <c r="D35">
+        <v>1.05131191880974E-3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>695</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C36">
+        <v>1.0608294799504401</v>
+      </c>
+      <c r="D36">
+        <v>1.2778793420155101E-3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>587</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1769</v>
+      </c>
+      <c r="C37">
+        <v>-1.2131988799148801</v>
+      </c>
+      <c r="D37">
+        <v>3.6136663728270602E-3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>631</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C38">
+        <v>-1.13529648447281</v>
+      </c>
+      <c r="D38">
+        <v>4.6671146506542501E-3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>-3.5045135684935498</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1.32233603142404E-55</v>
+      </c>
+      <c r="E39" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C40">
+        <v>-2.2868103650932898</v>
+      </c>
+      <c r="D40" s="1">
+        <v>8.5489467789449903E-27</v>
+      </c>
+      <c r="E40" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>922</v>
+      </c>
+      <c r="C41">
+        <v>-2.1334658367813901</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3.64159475163907E-23</v>
+      </c>
+      <c r="E41" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>323</v>
+      </c>
+      <c r="C42">
+        <v>2.3515349720062502</v>
+      </c>
+      <c r="D42" s="1">
+        <v>4.6938835034542499E-23</v>
+      </c>
+      <c r="E42" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>293</v>
+      </c>
+      <c r="C43">
+        <v>2.0779405387146701</v>
+      </c>
+      <c r="D43" s="1">
+        <v>6.1338979533654301E-21</v>
+      </c>
+      <c r="E43" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>-2.2821387380741198</v>
+      </c>
+      <c r="D44" s="1">
+        <v>3.2624775540480903E-20</v>
+      </c>
+      <c r="E44" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C45">
+        <v>-2.8898049751989499</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2.35382887594342E-18</v>
+      </c>
+      <c r="E45" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46">
+        <v>-1.7747004413554299</v>
+      </c>
+      <c r="D46" s="1">
+        <v>3.0528707945058897E-17</v>
+      </c>
+      <c r="E46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47">
+        <v>-1.55591553622964</v>
+      </c>
+      <c r="D47" s="1">
+        <v>3.0528707945058897E-17</v>
+      </c>
+      <c r="E47" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>385</v>
       </c>
-      <c r="B13">
+      <c r="C48">
         <v>-2.0359820723866799</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D48" s="1">
         <v>1.1450632324452501E-16</v>
       </c>
-      <c r="D13" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="E48" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B14">
+      <c r="C49">
         <v>2.2154617631671498</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D49" s="1">
         <v>1.18882792063138E-15</v>
       </c>
-      <c r="D14" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="E49" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>31</v>
       </c>
-      <c r="B15">
+      <c r="C50">
         <v>-2.00247068530759</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D50" s="1">
         <v>1.28683084446484E-15</v>
       </c>
-      <c r="D15" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="E50" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>1628</v>
       </c>
-      <c r="B16">
+      <c r="C51">
         <v>-3.0765737932121699</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D51" s="1">
         <v>2.5136509738263299E-15</v>
       </c>
-      <c r="D16" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="E51" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>456</v>
       </c>
-      <c r="B17">
+      <c r="C52">
         <v>1.7349681575650699</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D52" s="1">
         <v>3.3518811183111101E-15</v>
       </c>
-      <c r="D17" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="E52" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="C53">
         <v>1.7933144716139999</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D53" s="1">
         <v>7.0126723607025201E-14</v>
       </c>
-      <c r="D18" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>752</v>
-      </c>
-      <c r="B19">
-        <v>-1.86037036723702</v>
-      </c>
-      <c r="C19" s="1">
-        <v>3.54368218655103E-13</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>437</v>
-      </c>
-      <c r="B20">
-        <v>1.4858975462087101</v>
-      </c>
-      <c r="C20" s="1">
-        <v>4.8448382750820595E-13</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="E53" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>733</v>
       </c>
-      <c r="B21">
+      <c r="C54">
         <v>1.65546126012539</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D54" s="1">
         <v>1.1583316809878499E-12</v>
       </c>
-      <c r="D21" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="E54" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>1277</v>
       </c>
-      <c r="B22">
+      <c r="C55">
         <v>1.5473788122449901</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D55" s="1">
         <v>1.9614278014944399E-12</v>
       </c>
-      <c r="D22" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>1061</v>
-      </c>
-      <c r="B23">
-        <v>-1.7821926576200899</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1.9614278014944399E-12</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="E55" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>484</v>
       </c>
-      <c r="B24">
+      <c r="C56">
         <v>-1.9154494313741299</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D56" s="1">
         <v>1.1119962366499601E-11</v>
       </c>
-      <c r="D24" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25">
-        <v>-1.3288272014720399</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1.62658080002992E-11</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="E56" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>97</v>
       </c>
-      <c r="B26">
+      <c r="C57">
         <v>-1.62974659590857</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D57" s="1">
         <v>3.1298836023510797E-11</v>
       </c>
-      <c r="D26" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>1121</v>
-      </c>
-      <c r="B27">
-        <v>-2.8796573881859402</v>
-      </c>
-      <c r="C27" s="1">
-        <v>7.7775395089806197E-11</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="E57" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>1151</v>
       </c>
-      <c r="B28">
+      <c r="C58">
         <v>2.39217415672148</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D58" s="1">
         <v>4.4548947771833699E-10</v>
       </c>
-      <c r="D28" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="E58" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>540</v>
       </c>
-      <c r="B29">
+      <c r="C59">
         <v>-1.2910156905607599</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D59" s="1">
         <v>1.8626137748647901E-9</v>
       </c>
-      <c r="D29" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="E59" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>12</v>
       </c>
-      <c r="B30">
+      <c r="C60">
         <v>1.32674355131819</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D60" s="1">
         <v>1.88222678546165E-9</v>
       </c>
-      <c r="D30" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>1552</v>
-      </c>
-      <c r="B31">
-        <v>-2.0438599888878599</v>
-      </c>
-      <c r="C31" s="1">
-        <v>2.4220508604906199E-9</v>
-      </c>
-      <c r="D31" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32">
-        <v>-1.99255488807799</v>
-      </c>
-      <c r="C32" s="1">
-        <v>2.59906964508959E-9</v>
-      </c>
-      <c r="D32" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="E60" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>679</v>
       </c>
-      <c r="B33">
+      <c r="C61">
         <v>-2.08648846189769</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D61" s="1">
         <v>3.5686923090485501E-9</v>
       </c>
-      <c r="D33" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="E61" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>1237</v>
       </c>
-      <c r="B34">
+      <c r="C62">
         <v>-1.4207316251134601</v>
       </c>
-      <c r="C34" s="1">
+      <c r="D62" s="1">
         <v>4.0014564381676201E-8</v>
       </c>
-      <c r="D34" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="E62" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>10</v>
       </c>
-      <c r="B35">
+      <c r="C63">
         <v>1.1971168806353101</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D63" s="1">
         <v>4.7169760801922899E-8</v>
       </c>
-      <c r="D35" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>189</v>
-      </c>
-      <c r="B36">
-        <v>-1.1799194610025201</v>
-      </c>
-      <c r="C36" s="1">
-        <v>5.09438515353527E-8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="E63" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>491</v>
       </c>
-      <c r="B37">
+      <c r="C64">
         <v>1.32081000252256</v>
       </c>
-      <c r="C37" s="1">
+      <c r="D64" s="1">
         <v>7.4252250986903805E-8</v>
       </c>
-      <c r="D37" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="E64" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>332</v>
       </c>
-      <c r="B38">
+      <c r="C65">
         <v>1.16282993459606</v>
       </c>
-      <c r="C38" s="1">
+      <c r="D65" s="1">
         <v>1.1412638183831201E-7</v>
       </c>
-      <c r="D38" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="E65" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>519</v>
       </c>
-      <c r="B39">
+      <c r="C66">
         <v>-1.80576571509692</v>
       </c>
-      <c r="C39" s="1">
+      <c r="D66" s="1">
         <v>1.43831644091978E-7</v>
       </c>
-      <c r="D39" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>224</v>
-      </c>
-      <c r="B40">
-        <v>1.2461051126032201</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1.5011477666384201E-7</v>
-      </c>
-      <c r="D40" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="E66" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>61</v>
       </c>
-      <c r="B41">
+      <c r="C67">
         <v>1.08876448316868</v>
       </c>
-      <c r="C41" s="1">
+      <c r="D67" s="1">
         <v>2.3382332398411101E-7</v>
       </c>
-      <c r="D41" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="E67" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>997</v>
       </c>
-      <c r="B42">
+      <c r="C68">
         <v>-1.2551089619069</v>
       </c>
-      <c r="C42" s="1">
+      <c r="D68" s="1">
         <v>3.1559402767229802E-7</v>
       </c>
-      <c r="D42" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="E68" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>55</v>
       </c>
-      <c r="B43">
+      <c r="C69">
         <v>1.08975632039808</v>
       </c>
-      <c r="C43" s="1">
+      <c r="D69" s="1">
         <v>3.2628323577452001E-7</v>
       </c>
-      <c r="D43" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="E69" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>237</v>
       </c>
-      <c r="B44">
+      <c r="C70">
         <v>-2.0441189175721499</v>
       </c>
-      <c r="C44" s="1">
+      <c r="D70" s="1">
         <v>3.3406380885642602E-7</v>
       </c>
-      <c r="D44" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="E70" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>1235</v>
       </c>
-      <c r="B45">
+      <c r="C71">
         <v>-1.31145137537131</v>
       </c>
-      <c r="C45" s="1">
+      <c r="D71" s="1">
         <v>3.65689326551454E-7</v>
       </c>
-      <c r="D45" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>181</v>
-      </c>
-      <c r="B46">
-        <v>-1.2234421781558</v>
-      </c>
-      <c r="C46" s="1">
-        <v>3.9373922751673799E-7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47">
-        <v>1.0679696345156799</v>
-      </c>
-      <c r="C47" s="1">
-        <v>4.0667927823455498E-7</v>
-      </c>
-      <c r="D47" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="E71" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>765</v>
       </c>
-      <c r="B48">
+      <c r="C72">
         <v>-1.3235442774456501</v>
       </c>
-      <c r="C48" s="1">
+      <c r="D72" s="1">
         <v>7.2001458967529498E-7</v>
       </c>
-      <c r="D48" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49">
-        <v>1.0524700752590199</v>
-      </c>
-      <c r="C49" s="1">
-        <v>9.4937485745716404E-7</v>
-      </c>
-      <c r="D49" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="E72" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>1451</v>
       </c>
-      <c r="B50">
+      <c r="C73">
         <v>-1.4546481356232599</v>
       </c>
-      <c r="C50" s="1">
+      <c r="D73" s="1">
         <v>1.9499353614221498E-6</v>
       </c>
-      <c r="D50" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>1104</v>
-      </c>
-      <c r="B51">
-        <v>1.46455562637854</v>
-      </c>
-      <c r="C51" s="1">
-        <v>3.0289792320679399E-6</v>
-      </c>
-      <c r="D51" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>271</v>
-      </c>
-      <c r="B52">
-        <v>1.1959200342032299</v>
-      </c>
-      <c r="C52" s="1">
-        <v>3.55628518913805E-6</v>
-      </c>
-      <c r="D52" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="E73" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>376</v>
       </c>
-      <c r="B53">
+      <c r="C74">
         <v>-1.1669160456400001</v>
       </c>
-      <c r="C53" s="1">
+      <c r="D74" s="1">
         <v>3.58103912666505E-6</v>
       </c>
-      <c r="D53" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="E74" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>185</v>
       </c>
-      <c r="B54">
+      <c r="C75">
         <v>1.2288896043411399</v>
       </c>
-      <c r="C54" s="1">
+      <c r="D75" s="1">
         <v>4.31458421586163E-6</v>
       </c>
-      <c r="D54" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="E75" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>432</v>
       </c>
-      <c r="B55">
+      <c r="C76">
         <v>1.23658593459263</v>
       </c>
-      <c r="C55" s="1">
+      <c r="D76" s="1">
         <v>4.5962780683277797E-6</v>
       </c>
-      <c r="D55" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="E76" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>1380</v>
       </c>
-      <c r="B56">
+      <c r="C77">
         <v>-1.16452122791902</v>
       </c>
-      <c r="C56" s="1">
+      <c r="D77" s="1">
         <v>4.8253679236285097E-6</v>
       </c>
-      <c r="D56" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="E77" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>1405</v>
       </c>
-      <c r="B57">
+      <c r="C78">
         <v>1.4216084248571601</v>
       </c>
-      <c r="C57" s="1">
+      <c r="D78" s="1">
         <v>4.8827011831701101E-6</v>
       </c>
-      <c r="D57" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="E78" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>1518</v>
       </c>
-      <c r="B58">
+      <c r="C79">
         <v>-1.2955705576032199</v>
       </c>
-      <c r="C58" s="1">
+      <c r="D79" s="1">
         <v>5.6671142608234998E-6</v>
       </c>
-      <c r="D58" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="E79" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>1342</v>
       </c>
-      <c r="B59">
+      <c r="C80">
         <v>-1.43712839701576</v>
       </c>
-      <c r="C59" s="1">
+      <c r="D80" s="1">
         <v>5.8235576251907996E-6</v>
       </c>
-      <c r="D59" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>161</v>
-      </c>
-      <c r="B60">
-        <v>-1.0847203408766299</v>
-      </c>
-      <c r="C60" s="1">
-        <v>1.7155248462453598E-5</v>
-      </c>
-      <c r="D60" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>1216</v>
-      </c>
-      <c r="B61">
-        <v>-1.0217631192591801</v>
-      </c>
-      <c r="C61" s="1">
-        <v>2.3916407570055301E-5</v>
-      </c>
-      <c r="D61" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="E80" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>1467</v>
       </c>
-      <c r="B62">
+      <c r="C81">
         <v>1.6866466375217</v>
       </c>
-      <c r="C62" s="1">
+      <c r="D81" s="1">
         <v>2.74522042929354E-5</v>
       </c>
-      <c r="D62" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>49</v>
-      </c>
-      <c r="B63">
-        <v>2.3235159089566499</v>
-      </c>
-      <c r="C63" s="1">
-        <v>3.04325258625224E-5</v>
-      </c>
-      <c r="D63" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>1466</v>
-      </c>
-      <c r="B64">
-        <v>1.0204416778493699</v>
-      </c>
-      <c r="C64" s="1">
-        <v>3.3520452137941403E-5</v>
-      </c>
-      <c r="D64" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>1564</v>
-      </c>
-      <c r="B65">
-        <v>-1.12822436758008</v>
-      </c>
-      <c r="C65" s="1">
-        <v>3.6756536668956703E-5</v>
-      </c>
-      <c r="D65" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>1494</v>
-      </c>
-      <c r="B66">
-        <v>1.1432972758036</v>
-      </c>
-      <c r="C66" s="1">
-        <v>4.0796203427487102E-5</v>
-      </c>
-      <c r="D66" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>1184</v>
-      </c>
-      <c r="B67">
-        <v>1.0317782244409299</v>
-      </c>
-      <c r="C67" s="1">
+      <c r="E81" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>884</v>
+      </c>
+      <c r="C82">
+        <v>1.1878927772858801</v>
+      </c>
+      <c r="D82" s="1">
         <v>7.1645079986050697E-5</v>
       </c>
-      <c r="D67" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>884</v>
-      </c>
-      <c r="B68">
-        <v>1.1878927772858801</v>
-      </c>
-      <c r="C68" s="1">
-        <v>7.1645079986050697E-5</v>
-      </c>
-      <c r="D68" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>22</v>
-      </c>
-      <c r="B69">
-        <v>-1.3779073656566301</v>
-      </c>
-      <c r="C69" s="1">
-        <v>7.6231238054967797E-5</v>
-      </c>
-      <c r="D69" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>847</v>
-      </c>
-      <c r="B70">
-        <v>-1.1815399713377399</v>
-      </c>
-      <c r="C70" s="1">
-        <v>9.2788717779559198E-5</v>
-      </c>
-      <c r="D70" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="E82" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>569</v>
       </c>
-      <c r="B71">
+      <c r="C83">
         <v>1.11073464434881</v>
       </c>
-      <c r="C71">
+      <c r="D83">
         <v>1.2246612845037499E-4</v>
       </c>
-      <c r="D71" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>968</v>
-      </c>
-      <c r="B72">
-        <v>1.0039694740943701</v>
-      </c>
-      <c r="C72">
-        <v>1.23455357134426E-4</v>
-      </c>
-      <c r="D72" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>1594</v>
-      </c>
-      <c r="B73">
-        <v>-1.0422139202433001</v>
-      </c>
-      <c r="C73">
-        <v>1.3178587082486701E-4</v>
-      </c>
-      <c r="D73" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>1313</v>
-      </c>
-      <c r="B74">
-        <v>-1.0052650095943401</v>
-      </c>
-      <c r="C74">
-        <v>1.6277017857066399E-4</v>
-      </c>
-      <c r="D74" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="E83" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>1362</v>
       </c>
-      <c r="B75">
+      <c r="C84">
         <v>1.07539826179276</v>
       </c>
-      <c r="C75">
+      <c r="D84">
         <v>2.2223796766692399E-4</v>
       </c>
-      <c r="D75" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="E84" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>1105</v>
       </c>
-      <c r="B76">
+      <c r="C85">
         <v>-1.8780931347894101</v>
       </c>
-      <c r="C76">
+      <c r="D85">
         <v>2.70048388765063E-4</v>
       </c>
-      <c r="D76" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>1285</v>
-      </c>
-      <c r="B77">
-        <v>-1.00373648914888</v>
-      </c>
-      <c r="C77">
-        <v>2.8586141165042798E-4</v>
-      </c>
-      <c r="D77" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>440</v>
-      </c>
-      <c r="B78">
-        <v>-1.1173923333012199</v>
-      </c>
-      <c r="C78">
-        <v>2.86633308770816E-4</v>
-      </c>
-      <c r="D78" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="E85" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>1429</v>
       </c>
-      <c r="B79">
+      <c r="C86">
         <v>1.2081052019140599</v>
       </c>
-      <c r="C79">
+      <c r="D86">
         <v>3.8711637440407102E-4</v>
       </c>
-      <c r="D79" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="E86" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>1659</v>
       </c>
-      <c r="B80">
+      <c r="C87">
         <v>-1.36273734781161</v>
       </c>
-      <c r="C80">
+      <c r="D87">
         <v>5.2527183851769496E-4</v>
       </c>
-      <c r="D80" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>439</v>
-      </c>
-      <c r="B81">
-        <v>-1.47176509312627</v>
-      </c>
-      <c r="C81">
-        <v>6.4021010615734897E-4</v>
-      </c>
-      <c r="D81" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>1534</v>
-      </c>
-      <c r="B82">
-        <v>-1.04689807204282</v>
-      </c>
-      <c r="C82">
-        <v>7.7577589121875497E-4</v>
-      </c>
-      <c r="D82" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="E87" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>221</v>
       </c>
-      <c r="B83">
+      <c r="C88">
         <v>1.0479917229531099</v>
       </c>
-      <c r="C83">
+      <c r="D88">
         <v>8.1802060164261998E-4</v>
       </c>
-      <c r="D83" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>47</v>
-      </c>
-      <c r="B84">
-        <v>1.06762679466085</v>
-      </c>
-      <c r="C84">
-        <v>8.5783220937633105E-4</v>
-      </c>
-      <c r="D84" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>1418</v>
-      </c>
-      <c r="B85">
-        <v>-1.3034555548731801</v>
-      </c>
-      <c r="C85">
-        <v>1.05131191880974E-3</v>
-      </c>
-      <c r="D85" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>695</v>
-      </c>
-      <c r="B86">
-        <v>1.0608294799504401</v>
-      </c>
-      <c r="C86">
-        <v>1.2778793420155101E-3</v>
-      </c>
-      <c r="D86" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="E88" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>1071</v>
       </c>
-      <c r="B87">
+      <c r="C89">
         <v>-1.09766140928899</v>
       </c>
-      <c r="C87">
+      <c r="D89">
         <v>1.3774373748840999E-3</v>
       </c>
-      <c r="D87" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="E89" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>1649</v>
       </c>
-      <c r="B88">
+      <c r="C90">
         <v>1.0609027478369899</v>
       </c>
-      <c r="C88">
+      <c r="D90">
         <v>1.9404117171903999E-3</v>
       </c>
-      <c r="D88" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>587</v>
-      </c>
-      <c r="B89">
-        <v>-1.2131988799148801</v>
-      </c>
-      <c r="C89">
-        <v>3.6136663728270602E-3</v>
-      </c>
-      <c r="D89" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="E90" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>450</v>
       </c>
-      <c r="B90">
+      <c r="C91">
         <v>-1.01226824258509</v>
       </c>
-      <c r="C90">
+      <c r="D91">
         <v>4.3910269310246898E-3</v>
       </c>
-      <c r="D90" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="E91" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>199</v>
       </c>
-      <c r="B91">
+      <c r="C92">
         <v>1.00611416241316</v>
       </c>
-      <c r="C91">
+      <c r="D92">
         <v>4.4536662353960501E-3</v>
       </c>
-      <c r="D91" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>631</v>
-      </c>
-      <c r="B92">
-        <v>-1.13529648447281</v>
-      </c>
-      <c r="C92">
-        <v>4.6671146506542501E-3</v>
-      </c>
-      <c r="D92" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>82</v>
       </c>
-      <c r="B93">
+      <c r="C93">
         <v>1.30419043104568</v>
       </c>
-      <c r="C93">
+      <c r="D93">
         <v>7.8982366023641407E-3</v>
       </c>
-      <c r="D93" t="e">
+      <c r="E93" t="e">
         <v>#N/A</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E93">
+    <sortCondition ref="E2:E93"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>